<commit_message>
Import location and stable currency on sales report
</commit_message>
<xml_diff>
--- a/NatuurlikBase/NatuurlikBase/wwwroot/Uploads/Book1.xlsx
+++ b/NatuurlikBase/NatuurlikBase/wwwroot/Uploads/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292B8E0-FD67-41CF-8E5C-326936AF5EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9257DAD0-9CC7-4D9C-A67C-80CE3B1E2FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="2610" windowWidth="21600" windowHeight="11835" xr2:uid="{0F397AEF-E452-493C-A3FB-B550E9DF8F35}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F397AEF-E452-493C-A3FB-B550E9DF8F35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,52 +33,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Days</t>
+    <t>SuburbName</t>
   </si>
   <si>
-    <t>Value</t>
+    <t>PostalCode</t>
   </si>
   <si>
-    <t>Active</t>
+    <t>CityId</t>
   </si>
   <si>
-    <t>3 days</t>
-  </si>
-  <si>
-    <t>5 days</t>
-  </si>
-  <si>
-    <t>9 days</t>
-  </si>
-  <si>
-    <t>10 days</t>
-  </si>
-  <si>
-    <t>11 days</t>
-  </si>
-  <si>
-    <t>4 days</t>
-  </si>
-  <si>
-    <t>7 days</t>
-  </si>
-  <si>
-    <t>8 days</t>
+    <t>Hattflied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,13 +109,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F85A981-D5BF-4726-8002-103141935D34}" name="Table1" displayName="Table1" ref="A1:D10" totalsRowShown="0">
-  <autoFilter ref="A1:D10" xr:uid="{8F85A981-D5BF-4726-8002-103141935D34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F85A981-D5BF-4726-8002-103141935D34}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{8F85A981-D5BF-4726-8002-103141935D34}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{29505B2A-EFBD-4B60-A91C-B85B754B4C38}" name="Id"/>
-    <tableColumn id="2" xr3:uid="{45663EE1-61F8-47B3-9F02-2D44639F9FEE}" name="Days"/>
-    <tableColumn id="3" xr3:uid="{B076B603-7488-4381-B32A-A10FC262F843}" name="Value"/>
-    <tableColumn id="4" xr3:uid="{CE3EAE2B-CAF5-429A-9EF2-1E3D7A9190EC}" name="Active"/>
+    <tableColumn id="2" xr3:uid="{C2997D37-688F-4E7F-8914-5B8CFC3B659C}" name="SuburbName"/>
+    <tableColumn id="4" xr3:uid="{782D8F60-5D21-4D1A-9326-94ECEE902E0D}" name="PostalCode"/>
+    <tableColumn id="3" xr3:uid="{B076B603-7488-4381-B32A-A10FC262F843}" name="CityId"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -433,13 +418,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B53E2A1-97C5-4C77-B2EF-6BD6BFD587A1}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -457,134 +445,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="b">
+        <v>231</v>
+      </c>
+      <c r="D2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>9</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>22</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>